<commit_message>
update of database and plot-file
all work done on sunday ...
</commit_message>
<xml_diff>
--- a/Data_Process/Data_inputs/pump_diagram_aux_engine.xlsx
+++ b/Data_Process/Data_inputs/pump_diagram_aux_engine.xlsx
@@ -414,7 +414,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>500</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -450,52 +450,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.9672</c:v>
+                  <c:v>1.35408</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.3464</c:v>
+                  <c:v>6.084959999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.026400000000001</c:v>
+                  <c:v>8.436960000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.8376</c:v>
+                  <c:v>13.77264</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.1288</c:v>
+                  <c:v>28.18032</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.1568</c:v>
+                  <c:v>35.21952</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.2856</c:v>
+                  <c:v>42.39984</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36.2328</c:v>
+                  <c:v>50.72592</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.548</c:v>
+                  <c:v>56.7672</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>47.32560000000001</c:v>
+                  <c:v>66.25584000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>54.64560000000001</c:v>
+                  <c:v>76.50384000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>59.82</c:v>
+                  <c:v>83.748</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>64.2432</c:v>
+                  <c:v>89.94048</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>68.4648</c:v>
+                  <c:v>95.85072000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>72.3096</c:v>
+                  <c:v>101.23344</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>76.02</c:v>
+                  <c:v>106.428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -507,52 +507,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>15.68622222222222</c:v>
+                  <c:v>30.74499555555555</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.46622222222222</c:v>
+                  <c:v>30.31379555555556</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.40266666666666</c:v>
+                  <c:v>30.18922666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.15066666666667</c:v>
+                  <c:v>29.69530666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.43244444444444</c:v>
+                  <c:v>28.28759111111111</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.86755555555555</c:v>
+                  <c:v>27.18040888888889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.27555555555556</c:v>
+                  <c:v>26.02008888888889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.52755555555555</c:v>
+                  <c:v>24.5540088888889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.09688888888889</c:v>
+                  <c:v>23.70990222222222</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.372</c:v>
+                  <c:v>22.28912</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.36844444444444</c:v>
+                  <c:v>20.32215111111111</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.087555555555555</c:v>
+                  <c:v>17.8116088888889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.947555555555556</c:v>
+                  <c:v>15.57720888888889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.653777777777777</c:v>
+                  <c:v>13.04140444444445</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.502666666666666</c:v>
+                  <c:v>10.78522666666667</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.284</c:v>
+                  <c:v>8.39664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1055,7 +1055,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>400</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1091,67 +1091,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>9.012</c:v>
+                  <c:v>6.759</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.5808</c:v>
+                  <c:v>13.1856</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.148</c:v>
+                  <c:v>19.611</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.276</c:v>
+                  <c:v>24.957</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.7224</c:v>
+                  <c:v>31.2918</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49.39680000000001</c:v>
+                  <c:v>37.0476</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.9424</c:v>
+                  <c:v>43.4568</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.9696</c:v>
+                  <c:v>48.7272</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>73.63680000000001</c:v>
+                  <c:v>55.2276</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>81.63839999999999</c:v>
+                  <c:v>61.2288</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>89.8304</c:v>
+                  <c:v>67.3728</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>97.5408</c:v>
+                  <c:v>73.15560000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>105.988</c:v>
+                  <c:v>79.491</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>114.1008</c:v>
+                  <c:v>85.57560000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>123.012</c:v>
+                  <c:v>92.25899999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>131.5664</c:v>
+                  <c:v>98.6748</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>139.2848</c:v>
+                  <c:v>104.4636</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>145.5008</c:v>
+                  <c:v>109.1256</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>153.3288</c:v>
+                  <c:v>114.9966</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>159.476</c:v>
+                  <c:v>119.607</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>166.052</c:v>
+                  <c:v>124.539</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1163,67 +1163,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>18.6112</c:v>
+                  <c:v>10.4688</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.62656</c:v>
+                  <c:v>10.47744</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.63104</c:v>
+                  <c:v>10.47996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.6336</c:v>
+                  <c:v>10.4814</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.5312</c:v>
+                  <c:v>10.4238</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.4352</c:v>
+                  <c:v>10.3698</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.33344</c:v>
+                  <c:v>10.31256</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.19968</c:v>
+                  <c:v>10.23732</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.00256000000001</c:v>
+                  <c:v>10.12644</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17.81184</c:v>
+                  <c:v>10.01916</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.65504</c:v>
+                  <c:v>9.930959999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17.3248</c:v>
+                  <c:v>9.7452</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.83008</c:v>
+                  <c:v>9.46692</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16.42304</c:v>
+                  <c:v>9.23796</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15.90016</c:v>
+                  <c:v>8.94384</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.33824</c:v>
+                  <c:v>8.62776</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.784</c:v>
+                  <c:v>8.316</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.27136</c:v>
+                  <c:v>8.02764</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13.56992</c:v>
+                  <c:v>7.63308</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12.84864</c:v>
+                  <c:v>7.22736</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12.12032</c:v>
+                  <c:v>6.817679999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2851,7 +2851,7 @@
   <dimension ref="B6:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2861,13 +2861,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="2">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="3">
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
@@ -2916,11 +2916,11 @@
       </c>
       <c r="D9">
         <f>B9*$C$6/500</f>
-        <v>9.0120000000000005</v>
+        <v>6.7590000000000003</v>
       </c>
       <c r="E9">
         <f>C9*($C$6/500)^2</f>
-        <v>18.611200000000004</v>
+        <v>10.4688</v>
       </c>
       <c r="G9">
         <v>0.40300000000000002</v>
@@ -2934,11 +2934,11 @@
       </c>
       <c r="J9">
         <f>H9*$H$6/750</f>
-        <v>0.96720000000000017</v>
+        <v>1.3540800000000002</v>
       </c>
       <c r="K9">
         <f>I9*($H$6/750)^2</f>
-        <v>15.68622222222222</v>
+        <v>30.744995555555555</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
@@ -2950,11 +2950,11 @@
       </c>
       <c r="D10">
         <f t="shared" ref="D10:D29" si="0">B10*$C$6/500</f>
-        <v>17.5808</v>
+        <v>13.185599999999999</v>
       </c>
       <c r="E10">
         <f t="shared" ref="E10:E29" si="1">C10*($C$6/500)^2</f>
-        <v>18.626560000000001</v>
+        <v>10.47744</v>
       </c>
       <c r="G10">
         <v>1.8109999999999999</v>
@@ -2968,11 +2968,11 @@
       </c>
       <c r="J10">
         <f t="shared" ref="J10:J24" si="3">H10*$H$6/750</f>
-        <v>4.3464</v>
+        <v>6.0849599999999988</v>
       </c>
       <c r="K10">
         <f t="shared" ref="K10:K24" si="4">I10*($H$6/750)^2</f>
-        <v>15.466222222222221</v>
+        <v>30.313795555555558</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
@@ -2984,11 +2984,11 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>26.148</v>
+        <v>19.611000000000001</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>18.631040000000002</v>
+        <v>10.47996</v>
       </c>
       <c r="G11">
         <v>2.5110000000000001</v>
@@ -3002,11 +3002,11 @@
       </c>
       <c r="J11">
         <f t="shared" si="3"/>
-        <v>6.0264000000000006</v>
+        <v>8.4369600000000009</v>
       </c>
       <c r="K11">
         <f t="shared" si="4"/>
-        <v>15.402666666666665</v>
+        <v>30.189226666666666</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
@@ -3018,11 +3018,11 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>33.276000000000003</v>
+        <v>24.957000000000001</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>18.633600000000001</v>
+        <v>10.481399999999999</v>
       </c>
       <c r="G12">
         <v>4.0990000000000002</v>
@@ -3036,11 +3036,11 @@
       </c>
       <c r="J12">
         <f t="shared" si="3"/>
-        <v>9.8376000000000001</v>
+        <v>13.772640000000003</v>
       </c>
       <c r="K12">
         <f t="shared" si="4"/>
-        <v>15.150666666666666</v>
+        <v>29.695306666666667</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
@@ -3052,11 +3052,11 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>41.7224</v>
+        <v>31.291799999999999</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>18.531200000000002</v>
+        <v>10.423799999999998</v>
       </c>
       <c r="G13">
         <v>8.3870000000000005</v>
@@ -3070,11 +3070,11 @@
       </c>
       <c r="J13">
         <f t="shared" si="3"/>
-        <v>20.128800000000002</v>
+        <v>28.180320000000002</v>
       </c>
       <c r="K13">
         <f t="shared" si="4"/>
-        <v>14.432444444444442</v>
+        <v>28.287591111111112</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
@@ -3086,11 +3086,11 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>49.396800000000006</v>
+        <v>37.047599999999996</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>18.435200000000002</v>
+        <v>10.3698</v>
       </c>
       <c r="G14">
         <v>10.481999999999999</v>
@@ -3104,11 +3104,11 @@
       </c>
       <c r="J14">
         <f t="shared" si="3"/>
-        <v>25.156799999999997</v>
+        <v>35.219519999999996</v>
       </c>
       <c r="K14">
         <f t="shared" si="4"/>
-        <v>13.867555555555555</v>
+        <v>27.180408888888891</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
@@ -3120,11 +3120,11 @@
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>57.942399999999992</v>
+        <v>43.456799999999994</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>18.333440000000003</v>
+        <v>10.31256</v>
       </c>
       <c r="G15">
         <v>12.619</v>
@@ -3138,11 +3138,11 @@
       </c>
       <c r="J15">
         <f t="shared" si="3"/>
-        <v>30.285600000000002</v>
+        <v>42.399840000000005</v>
       </c>
       <c r="K15">
         <f t="shared" si="4"/>
-        <v>13.275555555555556</v>
+        <v>26.020088888888893</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
@@ -3154,11 +3154,11 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>64.9696</v>
+        <v>48.727200000000003</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>18.199680000000004</v>
+        <v>10.23732</v>
       </c>
       <c r="G16">
         <v>15.097</v>
@@ -3172,11 +3172,11 @@
       </c>
       <c r="J16">
         <f t="shared" si="3"/>
-        <v>36.232799999999997</v>
+        <v>50.725919999999995</v>
       </c>
       <c r="K16">
         <f t="shared" si="4"/>
-        <v>12.527555555555555</v>
+        <v>24.554008888888891</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
@@ -3188,11 +3188,11 @@
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>73.636800000000008</v>
+        <v>55.227600000000002</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>18.002560000000006</v>
+        <v>10.126440000000001</v>
       </c>
       <c r="G17">
         <v>16.895</v>
@@ -3206,11 +3206,11 @@
       </c>
       <c r="J17">
         <f t="shared" si="3"/>
-        <v>40.548000000000002</v>
+        <v>56.767200000000003</v>
       </c>
       <c r="K17">
         <f t="shared" si="4"/>
-        <v>12.096888888888888</v>
+        <v>23.709902222222222</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
@@ -3222,11 +3222,11 @@
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>81.63839999999999</v>
+        <v>61.2288</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>17.811840000000004</v>
+        <v>10.019159999999999</v>
       </c>
       <c r="G18">
         <v>19.719000000000001</v>
@@ -3240,11 +3240,11 @@
       </c>
       <c r="J18">
         <f t="shared" si="3"/>
-        <v>47.325600000000009</v>
+        <v>66.25584000000002</v>
       </c>
       <c r="K18">
         <f t="shared" si="4"/>
-        <v>11.372</v>
+        <v>22.28912</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
@@ -3256,11 +3256,11 @@
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>89.830399999999997</v>
+        <v>67.372799999999998</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>17.655040000000003</v>
+        <v>9.9309599999999989</v>
       </c>
       <c r="G19">
         <v>22.768999999999998</v>
@@ -3274,11 +3274,11 @@
       </c>
       <c r="J19">
         <f t="shared" si="3"/>
-        <v>54.645600000000009</v>
+        <v>76.503840000000011</v>
       </c>
       <c r="K19">
         <f t="shared" si="4"/>
-        <v>10.368444444444444</v>
+        <v>20.322151111111111</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
@@ -3290,11 +3290,11 @@
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>97.540800000000004</v>
+        <v>73.155600000000007</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>17.324800000000003</v>
+        <v>9.7452000000000005</v>
       </c>
       <c r="G20">
         <v>24.925000000000001</v>
@@ -3308,11 +3308,11 @@
       </c>
       <c r="J20">
         <f t="shared" si="3"/>
-        <v>59.82</v>
+        <v>83.748000000000005</v>
       </c>
       <c r="K20">
         <f t="shared" si="4"/>
-        <v>9.0875555555555554</v>
+        <v>17.811608888888891</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
@@ -3324,11 +3324,11 @@
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>105.98800000000001</v>
+        <v>79.491000000000014</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>16.830080000000002</v>
+        <v>9.46692</v>
       </c>
       <c r="G21">
         <v>26.768000000000001</v>
@@ -3342,11 +3342,11 @@
       </c>
       <c r="J21">
         <f t="shared" si="3"/>
-        <v>64.243200000000002</v>
+        <v>89.940479999999994</v>
       </c>
       <c r="K21">
         <f t="shared" si="4"/>
-        <v>7.9475555555555557</v>
+        <v>15.577208888888892</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
@@ -3358,11 +3358,11 @@
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>114.10080000000001</v>
+        <v>85.575600000000009</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>16.423040000000004</v>
+        <v>9.2379599999999993</v>
       </c>
       <c r="G22">
         <v>28.527000000000001</v>
@@ -3376,11 +3376,11 @@
       </c>
       <c r="J22">
         <f t="shared" si="3"/>
-        <v>68.464800000000011</v>
+        <v>95.85072000000001</v>
       </c>
       <c r="K22">
         <f t="shared" si="4"/>
-        <v>6.6537777777777771</v>
+        <v>13.041404444444446</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
@@ -3392,11 +3392,11 @@
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>123.01199999999999</v>
+        <v>92.258999999999986</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>15.900160000000003</v>
+        <v>8.9438399999999998</v>
       </c>
       <c r="G23">
         <v>30.129000000000001</v>
@@ -3410,11 +3410,11 @@
       </c>
       <c r="J23">
         <f t="shared" si="3"/>
-        <v>72.309600000000003</v>
+        <v>101.23344</v>
       </c>
       <c r="K23">
         <f t="shared" si="4"/>
-        <v>5.5026666666666664</v>
+        <v>10.785226666666668</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
@@ -3426,11 +3426,11 @@
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>131.56639999999999</v>
+        <v>98.674800000000005</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>15.338240000000004</v>
+        <v>8.6277600000000003</v>
       </c>
       <c r="G24">
         <v>31.675000000000001</v>
@@ -3444,11 +3444,11 @@
       </c>
       <c r="J24">
         <f t="shared" si="3"/>
-        <v>76.02</v>
+        <v>106.428</v>
       </c>
       <c r="K24">
         <f t="shared" si="4"/>
-        <v>4.2839999999999998</v>
+        <v>8.3966399999999997</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
@@ -3460,11 +3460,11 @@
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>139.28479999999999</v>
+        <v>104.46359999999999</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
-        <v>14.784000000000004</v>
+        <v>8.3160000000000007</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
@@ -3476,11 +3476,11 @@
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>145.50080000000003</v>
+        <v>109.12560000000001</v>
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
-        <v>14.271360000000003</v>
+        <v>8.0276399999999999</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
@@ -3492,11 +3492,11 @@
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>153.3288</v>
+        <v>114.9966</v>
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
-        <v>13.569920000000002</v>
+        <v>7.6330799999999996</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
@@ -3508,11 +3508,11 @@
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>159.476</v>
+        <v>119.607</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
-        <v>12.848640000000003</v>
+        <v>7.22736</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
@@ -3524,11 +3524,11 @@
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>166.05199999999999</v>
+        <v>124.539</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
-        <v>12.120320000000001</v>
+        <v>6.8176799999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>